<commit_message>
added files related Create purchase order
</commit_message>
<xml_diff>
--- a/CrmMAvenFrameWork/src/test/resources/testData.xlsx
+++ b/CrmMAvenFrameWork/src/test/resources/testData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8460" windowHeight="3675"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8460" windowHeight="3672" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="campaign" sheetId="1" r:id="rId1"/>
@@ -12,14 +12,14 @@
     <sheet name="conatct" sheetId="3" r:id="rId3"/>
     <sheet name="PRice" sheetId="4" r:id="rId4"/>
     <sheet name="so" sheetId="5" r:id="rId5"/>
+    <sheet name="createPO" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1:C7"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t>testID</t>
   </si>
@@ -74,12 +74,60 @@
   <si>
     <t>searchCompagin</t>
   </si>
+  <si>
+    <t>createPoTest</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>laptop</t>
+  </si>
+  <si>
+    <t>vendor</t>
+  </si>
+  <si>
+    <t>ABB</t>
+  </si>
+  <si>
+    <t>Billing Address</t>
+  </si>
+  <si>
+    <t>Bengaluru</t>
+  </si>
+  <si>
+    <t>Shipping Address</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>micro phone</t>
+  </si>
+  <si>
+    <t>qty</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>expected msg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Purchase Order Information </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,7 +150,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -125,14 +173,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -193,7 +254,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -225,10 +286,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -260,7 +320,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -436,21 +495,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -476,7 +535,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -491,7 +550,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -509,7 +568,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -525,7 +584,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -544,67 +603,180 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:2" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="130" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="130" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="130" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="27.21875" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" customWidth="1"/>
+    <col min="6" max="6" width="15.77734375" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" customWidth="1"/>
+    <col min="10" max="10" width="25.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
created AdminTest and created Admin Page in objectRespository and updated test/resources
</commit_message>
<xml_diff>
--- a/CrmMAvenFrameWork/src/test/resources/testData.xlsx
+++ b/CrmMAvenFrameWork/src/test/resources/testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8460" windowHeight="3672" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8460" windowHeight="3675" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="campaign" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,15 @@
     <sheet name="PRice" sheetId="4" r:id="rId4"/>
     <sheet name="so" sheetId="5" r:id="rId5"/>
     <sheet name="createPO" sheetId="6" r:id="rId6"/>
+    <sheet name="Quotes" sheetId="7" r:id="rId7"/>
+    <sheet name="Admin" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="80">
   <si>
     <t>testID</t>
   </si>
@@ -136,6 +138,129 @@
   </si>
   <si>
     <t>product</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Quotes</t>
+  </si>
+  <si>
+    <t>TestCase Number</t>
+  </si>
+  <si>
+    <t>TC_04</t>
+  </si>
+  <si>
+    <t>Quotes Name</t>
+  </si>
+  <si>
+    <t>Quotes Number</t>
+  </si>
+  <si>
+    <t>Search for</t>
+  </si>
+  <si>
+    <t>Search In</t>
+  </si>
+  <si>
+    <t>Filter_Name</t>
+  </si>
+  <si>
+    <t>Quote Info</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>equals</t>
+  </si>
+  <si>
+    <t>Opportunity Name</t>
+  </si>
+  <si>
+    <t>not equal to</t>
+  </si>
+  <si>
+    <t>Quote No</t>
+  </si>
+  <si>
+    <t>starts with</t>
+  </si>
+  <si>
+    <t>Quote Stage</t>
+  </si>
+  <si>
+    <t>ends with</t>
+  </si>
+  <si>
+    <t>Organization Name</t>
+  </si>
+  <si>
+    <t>contains</t>
+  </si>
+  <si>
+    <t>Assigned To</t>
+  </si>
+  <si>
+    <t>do not contains</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>TC_05</t>
+  </si>
+  <si>
+    <t>Organizations &amp; Contacts of</t>
+  </si>
+  <si>
+    <t>Accessed by</t>
+  </si>
+  <si>
+    <t>Permission</t>
+  </si>
+  <si>
+    <t>Read Only</t>
+  </si>
+  <si>
+    <t>Read/Write</t>
+  </si>
+  <si>
+    <t>Group::Team Selling</t>
+  </si>
+  <si>
+    <t>Group::Marketing Group</t>
+  </si>
+  <si>
+    <t>Group::Support Group</t>
+  </si>
+  <si>
+    <t>Roles::CEO</t>
+  </si>
+  <si>
+    <t>Roles::Vice President</t>
+  </si>
+  <si>
+    <t>Roles::Sales Manager</t>
+  </si>
+  <si>
+    <t>Roles::Sales Man</t>
+  </si>
+  <si>
+    <t>Roles and Subordinates::CEO</t>
+  </si>
+  <si>
+    <t>Roles and Subordinates::Vice President</t>
+  </si>
+  <si>
+    <t>Roles and Subordinates::Sales Manager</t>
+  </si>
+  <si>
+    <t>Roles and Subordinates::Sales Man</t>
   </si>
 </sst>
 </file>
@@ -203,27 +328,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -518,11 +642,11 @@
       <selection sqref="A1:H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -626,9 +750,9 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="43.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -646,7 +770,7 @@
   <sheetViews>
     <sheetView zoomScale="130" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -660,7 +784,7 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -674,7 +798,7 @@
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -684,19 +808,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="27.21875" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" customWidth="1"/>
-    <col min="6" max="6" width="15.77734375" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" customWidth="1"/>
-    <col min="10" max="10" width="25.5546875" customWidth="1"/>
-    <col min="11" max="11" width="11.5546875" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="10" max="10" width="25.5703125" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -827,4 +951,458 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+    </row>
+    <row r="2" spans="1:9" ht="30">
+      <c r="A2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="30">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:O13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="43.7109375" customWidth="1"/>
+    <col min="4" max="4" width="41.5703125" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>